<commit_message>
Fix of bug in structure of stairway / stair
</commit_message>
<xml_diff>
--- a/conceptlist.xlsx
+++ b/conceptlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\atlantis_public\indoor_object_taxonomy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\atlantis\atlantis_git\IndoorObjectTaxonomy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5108" uniqueCount="2822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5108" uniqueCount="2823">
   <si>
     <t>Label</t>
   </si>
@@ -7229,9 +7229,6 @@
     <t>stairs</t>
   </si>
   <si>
-    <t>http://scan-net.org/concepts/stairs</t>
-  </si>
-  <si>
     <t>stairway.n.01</t>
   </si>
   <si>
@@ -8490,6 +8487,12 @@
   </si>
   <si>
     <t>broom.n.02</t>
+  </si>
+  <si>
+    <t>stairway</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/2006/03/wn/wn20/instances/synset-stairway-noun-01</t>
   </si>
 </sst>
 </file>
@@ -8809,8 +8812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1087"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="A1:L1087"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="K145" sqref="K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12155,22 +12158,19 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>2400</v>
+        <v>2821</v>
       </c>
       <c r="B143">
         <v>58</v>
       </c>
       <c r="C143" t="s">
-        <v>2401</v>
-      </c>
-      <c r="D143" t="s">
-        <v>2400</v>
+        <v>2402</v>
       </c>
       <c r="F143">
         <v>38</v>
       </c>
       <c r="J143" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="K143" t="s">
         <v>31</v>
@@ -12187,13 +12187,16 @@
         <v>2963</v>
       </c>
       <c r="C144" t="s">
+        <v>2822</v>
+      </c>
+      <c r="D144" t="s">
+        <v>2400</v>
+      </c>
+      <c r="J144" t="s">
         <v>2403</v>
       </c>
-      <c r="J144" t="s">
-        <v>2404</v>
-      </c>
       <c r="K144" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L144">
         <v>7</v>
@@ -12416,16 +12419,16 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="B155">
         <v>1209</v>
       </c>
       <c r="C155" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D155" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="F155">
         <v>39</v>
@@ -12442,16 +12445,16 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="B156">
         <v>2964</v>
       </c>
       <c r="C156" t="s">
+        <v>2407</v>
+      </c>
+      <c r="J156" t="s">
         <v>2408</v>
-      </c>
-      <c r="J156" t="s">
-        <v>2409</v>
       </c>
       <c r="K156" t="s">
         <v>31</v>
@@ -12462,16 +12465,16 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="B157">
         <v>2965</v>
       </c>
       <c r="C157" t="s">
+        <v>2410</v>
+      </c>
+      <c r="J157" t="s">
         <v>2411</v>
-      </c>
-      <c r="J157" t="s">
-        <v>2412</v>
       </c>
       <c r="K157" t="s">
         <v>15</v>
@@ -12482,16 +12485,16 @@
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="B158">
         <v>2966</v>
       </c>
       <c r="C158" t="s">
+        <v>2413</v>
+      </c>
+      <c r="J158" t="s">
         <v>2414</v>
-      </c>
-      <c r="J158" t="s">
-        <v>2415</v>
       </c>
       <c r="K158" t="s">
         <v>15</v>
@@ -12502,22 +12505,22 @@
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="B159">
         <v>1172</v>
       </c>
       <c r="C159" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="D159" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="F159">
         <v>40</v>
       </c>
       <c r="J159" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="K159" t="s">
         <v>31</v>
@@ -12612,22 +12615,22 @@
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="B163">
         <v>1194</v>
       </c>
       <c r="C163" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="D163" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="F163">
         <v>40</v>
       </c>
       <c r="J163" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="K163" t="s">
         <v>31</v>
@@ -14245,10 +14248,10 @@
         <v>2968</v>
       </c>
       <c r="C225" t="s">
+        <v>2420</v>
+      </c>
+      <c r="J225" t="s">
         <v>2421</v>
-      </c>
-      <c r="J225" t="s">
-        <v>2422</v>
       </c>
       <c r="K225" t="s">
         <v>15</v>
@@ -14259,25 +14262,25 @@
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="B226">
         <v>48</v>
       </c>
       <c r="C226" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="D226" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="F226">
         <v>40</v>
       </c>
       <c r="H226" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="J226" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="K226" t="s">
         <v>31</v>
@@ -14288,22 +14291,22 @@
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="B227">
         <v>570</v>
       </c>
       <c r="C227" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="D227" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="F227">
         <v>37</v>
       </c>
       <c r="J227" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="K227" t="s">
         <v>31</v>
@@ -14314,16 +14317,16 @@
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="B228">
         <v>1252</v>
       </c>
       <c r="C228" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="D228" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="F228">
         <v>37</v>
@@ -14332,7 +14335,7 @@
         <v>201</v>
       </c>
       <c r="J228" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="K228" t="s">
         <v>31</v>
@@ -14343,22 +14346,22 @@
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="B229">
         <v>1072</v>
       </c>
       <c r="C229" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D229" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="F229">
         <v>37</v>
       </c>
       <c r="J229" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="K229" t="s">
         <v>31</v>
@@ -14369,22 +14372,22 @@
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="B230">
         <v>1227</v>
       </c>
       <c r="C230" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="D230" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="F230">
         <v>39</v>
       </c>
       <c r="J230" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="K230" t="s">
         <v>31</v>
@@ -14395,16 +14398,16 @@
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="B231">
         <v>1230</v>
       </c>
       <c r="C231" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="D231" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="F231">
         <v>37</v>
@@ -14418,22 +14421,22 @@
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="B232">
         <v>1231</v>
       </c>
       <c r="C232" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="D232" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="F232">
         <v>40</v>
       </c>
       <c r="J232" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="K232" t="s">
         <v>31</v>
@@ -14444,22 +14447,22 @@
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="B233">
         <v>1234</v>
       </c>
       <c r="C233" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="D233" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="F233">
         <v>40</v>
       </c>
       <c r="J233" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="K233" t="s">
         <v>31</v>
@@ -14470,16 +14473,16 @@
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="B234">
         <v>1264</v>
       </c>
       <c r="C234" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="D234" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="F234">
         <v>37</v>
@@ -14488,7 +14491,7 @@
         <v>201</v>
       </c>
       <c r="J234" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="K234" t="s">
         <v>31</v>
@@ -14499,16 +14502,16 @@
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="B235">
         <v>440</v>
       </c>
       <c r="C235" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="D235" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="F235">
         <v>37</v>
@@ -14525,22 +14528,22 @@
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="B236">
         <v>480</v>
       </c>
       <c r="C236" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="D236" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="F236">
         <v>37</v>
       </c>
       <c r="J236" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="K236" t="s">
         <v>31</v>
@@ -14551,22 +14554,22 @@
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="B237">
         <v>506</v>
       </c>
       <c r="C237" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="D237" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="F237">
         <v>37</v>
       </c>
       <c r="J237" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="K237" t="s">
         <v>31</v>
@@ -14577,16 +14580,16 @@
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="B238">
         <v>1354</v>
       </c>
       <c r="C238" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="D238" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="F238">
         <v>40</v>
@@ -14600,16 +14603,16 @@
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="B239">
         <v>1356</v>
       </c>
       <c r="C239" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="D239" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="F239">
         <v>37</v>
@@ -14623,16 +14626,16 @@
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="B240">
         <v>2969</v>
       </c>
       <c r="C240" t="s">
+        <v>2460</v>
+      </c>
+      <c r="J240" t="s">
         <v>2461</v>
-      </c>
-      <c r="J240" t="s">
-        <v>2462</v>
       </c>
       <c r="K240" t="s">
         <v>15</v>
@@ -14643,22 +14646,22 @@
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="B241">
         <v>1297</v>
       </c>
       <c r="C241" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="D241" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="F241">
         <v>37</v>
       </c>
       <c r="J241" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="K241" t="s">
         <v>31</v>
@@ -14675,10 +14678,10 @@
         <v>2970</v>
       </c>
       <c r="C242" t="s">
+        <v>2465</v>
+      </c>
+      <c r="J242" t="s">
         <v>2466</v>
-      </c>
-      <c r="J242" t="s">
-        <v>2467</v>
       </c>
       <c r="K242" t="s">
         <v>15</v>
@@ -14689,28 +14692,28 @@
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="B243">
         <v>65</v>
       </c>
       <c r="C243" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="D243" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="F243">
         <v>40</v>
       </c>
       <c r="G243" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="H243" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J243" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K243" t="s">
         <v>31</v>
@@ -14721,25 +14724,25 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="B244">
         <v>392</v>
       </c>
       <c r="C244" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="D244" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="F244">
         <v>40</v>
       </c>
       <c r="G244" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J244" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="K244" t="s">
         <v>31</v>
@@ -14750,16 +14753,16 @@
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="B245">
         <v>2971</v>
       </c>
       <c r="C245" t="s">
+        <v>2474</v>
+      </c>
+      <c r="J245" t="s">
         <v>2475</v>
-      </c>
-      <c r="J245" t="s">
-        <v>2476</v>
       </c>
       <c r="K245" t="s">
         <v>15</v>
@@ -14770,16 +14773,16 @@
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="B246">
         <v>2972</v>
       </c>
       <c r="C246" t="s">
+        <v>2477</v>
+      </c>
+      <c r="J246" t="s">
         <v>2478</v>
-      </c>
-      <c r="J246" t="s">
-        <v>2479</v>
       </c>
       <c r="K246" t="s">
         <v>15</v>
@@ -14790,25 +14793,25 @@
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="B247">
         <v>726</v>
       </c>
       <c r="C247" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="D247" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="F247">
         <v>40</v>
       </c>
       <c r="G247" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J247" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="K247" t="s">
         <v>31</v>
@@ -14880,22 +14883,22 @@
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="B250">
         <v>488</v>
       </c>
       <c r="C250" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="D250" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="F250">
         <v>40</v>
       </c>
       <c r="J250" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="K250" t="s">
         <v>31</v>
@@ -14912,7 +14915,7 @@
         <v>919</v>
       </c>
       <c r="C251" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="D251" t="s">
         <v>1024</v>
@@ -14924,7 +14927,7 @@
         <v>1024</v>
       </c>
       <c r="J251" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="K251" t="s">
         <v>31</v>
@@ -15002,25 +15005,25 @@
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="B254">
         <v>1206</v>
       </c>
       <c r="C254" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="D254" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="F254">
         <v>40</v>
       </c>
       <c r="G254" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J254" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K254" t="s">
         <v>31</v>
@@ -15031,22 +15034,22 @@
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="B255">
         <v>226</v>
       </c>
       <c r="C255" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="D255" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="F255">
         <v>40</v>
       </c>
       <c r="J255" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="K255" t="s">
         <v>31</v>
@@ -15057,22 +15060,22 @@
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="B256">
         <v>1176</v>
       </c>
       <c r="C256" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="D256" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="F256">
         <v>40</v>
       </c>
       <c r="J256" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="K256" t="s">
         <v>31</v>
@@ -15083,22 +15086,22 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B257">
         <v>1309</v>
       </c>
       <c r="C257" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="D257" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="F257">
         <v>40</v>
       </c>
       <c r="J257" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="K257" t="s">
         <v>31</v>
@@ -15109,22 +15112,22 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B258">
         <v>621</v>
       </c>
       <c r="C258" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="D258" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="F258">
         <v>40</v>
       </c>
       <c r="J258" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="K258" t="s">
         <v>31</v>
@@ -15135,22 +15138,22 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="B259">
         <v>997</v>
       </c>
       <c r="C259" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="D259" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="F259">
         <v>40</v>
       </c>
       <c r="J259" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="K259" t="s">
         <v>31</v>
@@ -15161,22 +15164,22 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="B260">
         <v>1222</v>
       </c>
       <c r="C260" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="D260" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="F260">
         <v>40</v>
       </c>
       <c r="J260" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="K260" t="s">
         <v>31</v>
@@ -15187,25 +15190,25 @@
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="B261">
         <v>1228</v>
       </c>
       <c r="C261" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="D261" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="F261">
         <v>40</v>
       </c>
       <c r="G261" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J261" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K261" t="s">
         <v>31</v>
@@ -15216,22 +15219,22 @@
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="B262">
         <v>1229</v>
       </c>
       <c r="C262" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="D262" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F262">
         <v>40</v>
       </c>
       <c r="J262" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K262" t="s">
         <v>31</v>
@@ -15242,25 +15245,25 @@
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="B263">
         <v>167</v>
       </c>
       <c r="C263" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="D263" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="F263">
         <v>40</v>
       </c>
       <c r="G263" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J263" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K263" t="s">
         <v>31</v>
@@ -15271,22 +15274,22 @@
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="B264">
         <v>563</v>
       </c>
       <c r="C264" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="D264" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="F264">
         <v>40</v>
       </c>
       <c r="J264" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="K264" t="s">
         <v>31</v>
@@ -15297,25 +15300,25 @@
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="B265">
         <v>1262</v>
       </c>
       <c r="C265" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="D265" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="F265">
         <v>40</v>
       </c>
       <c r="G265" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J265" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K265" t="s">
         <v>31</v>
@@ -15326,25 +15329,25 @@
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="B266">
         <v>1279</v>
       </c>
       <c r="C266" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="D266" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="F266">
         <v>40</v>
       </c>
       <c r="G266" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J266" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K266" t="s">
         <v>31</v>
@@ -15355,25 +15358,25 @@
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B267">
         <v>1304</v>
       </c>
       <c r="C267" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="D267" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="F267">
         <v>40</v>
       </c>
       <c r="G267" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J267" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K267" t="s">
         <v>31</v>
@@ -15384,25 +15387,25 @@
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B268">
         <v>1308</v>
       </c>
       <c r="C268" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="D268" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="F268">
         <v>40</v>
       </c>
       <c r="G268" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J268" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K268" t="s">
         <v>31</v>
@@ -15413,25 +15416,25 @@
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="B269">
         <v>1324</v>
       </c>
       <c r="C269" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="D269" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="F269">
         <v>40</v>
       </c>
       <c r="G269" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="J269" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="K269" t="s">
         <v>31</v>
@@ -15442,16 +15445,16 @@
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="B270">
         <v>1346</v>
       </c>
       <c r="C270" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="D270" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="F270">
         <v>40</v>
@@ -15460,7 +15463,7 @@
         <v>1024</v>
       </c>
       <c r="J270" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="K270" t="s">
         <v>31</v>
@@ -15471,22 +15474,22 @@
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="B271">
         <v>397</v>
       </c>
       <c r="C271" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="D271" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="F271">
         <v>40</v>
       </c>
       <c r="J271" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K271" t="s">
         <v>31</v>
@@ -15526,16 +15529,16 @@
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="B273">
         <v>2973</v>
       </c>
       <c r="C273" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="E273" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="J273" t="s">
         <v>831</v>
@@ -15549,16 +15552,16 @@
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="B274">
         <v>2974</v>
       </c>
       <c r="C274" t="s">
+        <v>2532</v>
+      </c>
+      <c r="J274" t="s">
         <v>2533</v>
-      </c>
-      <c r="J274" t="s">
-        <v>2534</v>
       </c>
       <c r="K274" t="s">
         <v>15</v>
@@ -15633,16 +15636,16 @@
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="B277">
         <v>1269</v>
       </c>
       <c r="C277" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="D277" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="F277">
         <v>40</v>
@@ -15662,16 +15665,16 @@
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="B278">
         <v>1357</v>
       </c>
       <c r="C278" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="D278" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="F278">
         <v>40</v>
@@ -15691,16 +15694,16 @@
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="B279">
         <v>2975</v>
       </c>
       <c r="C279" t="s">
+        <v>2539</v>
+      </c>
+      <c r="J279" t="s">
         <v>2540</v>
-      </c>
-      <c r="J279" t="s">
-        <v>2541</v>
       </c>
       <c r="K279" t="s">
         <v>15</v>
@@ -15924,16 +15927,16 @@
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="B289">
         <v>2979</v>
       </c>
       <c r="C289" t="s">
+        <v>2542</v>
+      </c>
+      <c r="J289" t="s">
         <v>2543</v>
-      </c>
-      <c r="J289" t="s">
-        <v>2544</v>
       </c>
       <c r="K289" t="s">
         <v>15</v>
@@ -15944,22 +15947,22 @@
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="B290">
         <v>185</v>
       </c>
       <c r="C290" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="D290" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="F290">
         <v>40</v>
       </c>
       <c r="J290" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="K290" t="s">
         <v>31</v>
@@ -15970,22 +15973,22 @@
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="B291">
         <v>356</v>
       </c>
       <c r="C291" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="D291" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="F291">
         <v>40</v>
       </c>
       <c r="J291" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="K291" t="s">
         <v>31</v>
@@ -15996,16 +15999,16 @@
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="B292">
         <v>2980</v>
       </c>
       <c r="C292" t="s">
+        <v>2551</v>
+      </c>
+      <c r="J292" t="s">
         <v>2552</v>
-      </c>
-      <c r="J292" t="s">
-        <v>2553</v>
       </c>
       <c r="K292" t="s">
         <v>15</v>
@@ -16051,16 +16054,16 @@
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="B294">
         <v>2981</v>
       </c>
       <c r="C294" t="s">
+        <v>2554</v>
+      </c>
+      <c r="J294" t="s">
         <v>2555</v>
-      </c>
-      <c r="J294" t="s">
-        <v>2556</v>
       </c>
       <c r="K294" t="s">
         <v>15</v>
@@ -16071,22 +16074,22 @@
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="B295">
         <v>1207</v>
       </c>
       <c r="C295" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="D295" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="F295">
         <v>40</v>
       </c>
       <c r="J295" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="K295" t="s">
         <v>31</v>
@@ -16360,16 +16363,16 @@
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="B306">
         <v>2982</v>
       </c>
       <c r="C306" t="s">
+        <v>2560</v>
+      </c>
+      <c r="J306" t="s">
         <v>2561</v>
-      </c>
-      <c r="J306" t="s">
-        <v>2562</v>
       </c>
       <c r="K306" t="s">
         <v>15</v>
@@ -16380,22 +16383,22 @@
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="B307">
         <v>1170</v>
       </c>
       <c r="C307" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="D307" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="F307">
         <v>40</v>
       </c>
       <c r="J307" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="K307" t="s">
         <v>31</v>
@@ -16406,16 +16409,16 @@
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="B308">
         <v>2983</v>
       </c>
       <c r="C308" t="s">
+        <v>2566</v>
+      </c>
+      <c r="J308" t="s">
         <v>2567</v>
-      </c>
-      <c r="J308" t="s">
-        <v>2568</v>
       </c>
       <c r="K308" t="s">
         <v>15</v>
@@ -16646,16 +16649,16 @@
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="B320">
         <v>2984</v>
       </c>
       <c r="C320" t="s">
+        <v>2569</v>
+      </c>
+      <c r="J320" t="s">
         <v>2570</v>
-      </c>
-      <c r="J320" t="s">
-        <v>2571</v>
       </c>
       <c r="K320" t="s">
         <v>15</v>
@@ -16666,25 +16669,25 @@
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="B321">
         <v>101</v>
       </c>
       <c r="C321" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="D321" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="F321">
         <v>40</v>
       </c>
       <c r="G321" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="J321" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="K321" t="s">
         <v>31</v>
@@ -16695,16 +16698,16 @@
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="B322">
         <v>2985</v>
       </c>
       <c r="C322" t="s">
+        <v>2575</v>
+      </c>
+      <c r="J322" t="s">
         <v>2576</v>
-      </c>
-      <c r="J322" t="s">
-        <v>2577</v>
       </c>
       <c r="K322" t="s">
         <v>15</v>
@@ -16715,19 +16718,19 @@
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="B323">
         <v>2043</v>
       </c>
       <c r="C323" t="s">
+        <v>2578</v>
+      </c>
+      <c r="H323" t="s">
+        <v>2577</v>
+      </c>
+      <c r="J323" t="s">
         <v>2579</v>
-      </c>
-      <c r="H323" t="s">
-        <v>2578</v>
-      </c>
-      <c r="J323" t="s">
-        <v>2580</v>
       </c>
       <c r="K323" t="s">
         <v>31</v>
@@ -16738,16 +16741,16 @@
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="B324">
         <v>2986</v>
       </c>
       <c r="C324" t="s">
+        <v>2581</v>
+      </c>
+      <c r="J324" t="s">
         <v>2582</v>
-      </c>
-      <c r="J324" t="s">
-        <v>2583</v>
       </c>
       <c r="K324" t="s">
         <v>15</v>
@@ -16758,16 +16761,16 @@
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="B325">
         <v>2987</v>
       </c>
       <c r="C325" t="s">
+        <v>2584</v>
+      </c>
+      <c r="J325" t="s">
         <v>2585</v>
-      </c>
-      <c r="J325" t="s">
-        <v>2586</v>
       </c>
       <c r="K325" t="s">
         <v>15</v>
@@ -16836,16 +16839,16 @@
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="B328">
         <v>2988</v>
       </c>
       <c r="C328" t="s">
+        <v>2587</v>
+      </c>
+      <c r="J328" t="s">
         <v>2588</v>
-      </c>
-      <c r="J328" t="s">
-        <v>2589</v>
       </c>
       <c r="K328" t="s">
         <v>15</v>
@@ -16856,22 +16859,22 @@
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="B329">
         <v>72</v>
       </c>
       <c r="C329" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="D329" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="F329">
         <v>40</v>
       </c>
       <c r="J329" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="K329" t="s">
         <v>31</v>
@@ -16905,19 +16908,19 @@
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="B331">
         <v>2596</v>
       </c>
       <c r="C331" t="s">
+        <v>2593</v>
+      </c>
+      <c r="I331" t="s">
+        <v>2592</v>
+      </c>
+      <c r="J331" t="s">
         <v>2594</v>
-      </c>
-      <c r="I331" t="s">
-        <v>2593</v>
-      </c>
-      <c r="J331" t="s">
-        <v>2595</v>
       </c>
       <c r="K331" t="s">
         <v>31</v>
@@ -16934,7 +16937,7 @@
         <v>2200</v>
       </c>
       <c r="C332" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="I332" t="s">
         <v>463</v>
@@ -16954,7 +16957,7 @@
         <v>2414</v>
       </c>
       <c r="C333" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="I333" t="s">
         <v>472</v>
@@ -16968,16 +16971,16 @@
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="B334">
         <v>2648</v>
       </c>
       <c r="C334" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="I334" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="K334" t="s">
         <v>31</v>
@@ -16988,16 +16991,16 @@
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="B335">
         <v>2167</v>
       </c>
       <c r="C335" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="I335" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="K335" t="s">
         <v>31</v>
@@ -17008,16 +17011,16 @@
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B336">
         <v>2515</v>
       </c>
       <c r="C336" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="I336" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="K336" t="s">
         <v>31</v>
@@ -17028,16 +17031,16 @@
     </row>
     <row r="337" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="B337">
         <v>2910</v>
       </c>
       <c r="C337" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="I337" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="K337" t="s">
         <v>31</v>
@@ -17077,16 +17080,16 @@
     </row>
     <row r="339" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="B339">
         <v>2712</v>
       </c>
       <c r="C339" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="I339" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="K339" t="s">
         <v>31</v>
@@ -17097,16 +17100,16 @@
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="B340">
         <v>2771</v>
       </c>
       <c r="C340" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="I340" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="K340" t="s">
         <v>31</v>
@@ -17146,16 +17149,16 @@
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="B342">
         <v>2989</v>
       </c>
       <c r="C342" t="s">
+        <v>2610</v>
+      </c>
+      <c r="J342" t="s">
         <v>2611</v>
-      </c>
-      <c r="J342" t="s">
-        <v>2612</v>
       </c>
       <c r="K342" t="s">
         <v>15</v>
@@ -17166,22 +17169,22 @@
     </row>
     <row r="343" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="B343">
         <v>1212</v>
       </c>
       <c r="C343" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="D343" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="F343">
         <v>40</v>
       </c>
       <c r="J343" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="K343" t="s">
         <v>31</v>
@@ -17192,16 +17195,16 @@
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="B344">
         <v>2990</v>
       </c>
       <c r="C344" t="s">
+        <v>2616</v>
+      </c>
+      <c r="J344" t="s">
         <v>2617</v>
-      </c>
-      <c r="J344" t="s">
-        <v>2618</v>
       </c>
       <c r="K344" t="s">
         <v>15</v>
@@ -17218,7 +17221,7 @@
         <v>168</v>
       </c>
       <c r="C345" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="D345" t="s">
         <v>2388</v>
@@ -17227,7 +17230,7 @@
         <v>40</v>
       </c>
       <c r="J345" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="K345" t="s">
         <v>31</v>
@@ -17267,16 +17270,16 @@
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="B347">
         <v>2991</v>
       </c>
       <c r="C347" t="s">
+        <v>2621</v>
+      </c>
+      <c r="J347" t="s">
         <v>2622</v>
-      </c>
-      <c r="J347" t="s">
-        <v>2623</v>
       </c>
       <c r="K347" t="s">
         <v>15</v>
@@ -17287,22 +17290,22 @@
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="B348">
         <v>1266</v>
       </c>
       <c r="C348" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="D348" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="F348">
         <v>40</v>
       </c>
       <c r="J348" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="K348" t="s">
         <v>31</v>
@@ -17875,16 +17878,16 @@
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="B369">
         <v>2993</v>
       </c>
       <c r="C369" t="s">
+        <v>2627</v>
+      </c>
+      <c r="J369" t="s">
         <v>2628</v>
-      </c>
-      <c r="J369" t="s">
-        <v>2629</v>
       </c>
       <c r="K369" t="s">
         <v>15</v>
@@ -20302,16 +20305,16 @@
     </row>
     <row r="474" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="B474">
         <v>3006</v>
       </c>
       <c r="C474" t="s">
+        <v>2630</v>
+      </c>
+      <c r="J474" t="s">
         <v>2631</v>
-      </c>
-      <c r="J474" t="s">
-        <v>2632</v>
       </c>
       <c r="K474" t="s">
         <v>15</v>
@@ -20721,16 +20724,16 @@
     </row>
     <row r="493" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="B493">
         <v>494</v>
       </c>
       <c r="C493" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="D493" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="F493">
         <v>4</v>
@@ -20750,16 +20753,16 @@
     </row>
     <row r="494" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="B494">
         <v>3009</v>
       </c>
       <c r="C494" t="s">
+        <v>2635</v>
+      </c>
+      <c r="J494" t="s">
         <v>2636</v>
-      </c>
-      <c r="J494" t="s">
-        <v>2637</v>
       </c>
       <c r="K494" t="s">
         <v>15</v>
@@ -20770,16 +20773,16 @@
     </row>
     <row r="495" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="B495">
         <v>75</v>
       </c>
       <c r="C495" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="D495" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="F495">
         <v>3</v>
@@ -20788,7 +20791,7 @@
         <v>419</v>
       </c>
       <c r="J495" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="K495" t="s">
         <v>31</v>
@@ -20799,16 +20802,16 @@
     </row>
     <row r="496" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="B496">
         <v>592</v>
       </c>
       <c r="C496" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="D496" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="F496">
         <v>40</v>
@@ -20822,16 +20825,16 @@
     </row>
     <row r="497" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="B497">
         <v>813</v>
       </c>
       <c r="C497" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="D497" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="F497">
         <v>40</v>
@@ -20845,16 +20848,16 @@
     </row>
     <row r="498" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="B498">
         <v>3010</v>
       </c>
       <c r="C498" t="s">
+        <v>2645</v>
+      </c>
+      <c r="J498" t="s">
         <v>2646</v>
-      </c>
-      <c r="J498" t="s">
-        <v>2647</v>
       </c>
       <c r="K498" t="s">
         <v>15</v>
@@ -20865,22 +20868,22 @@
     </row>
     <row r="499" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="B499">
         <v>51</v>
       </c>
       <c r="C499" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D499" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="F499">
         <v>39</v>
       </c>
       <c r="J499" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="K499" t="s">
         <v>31</v>
@@ -20891,16 +20894,16 @@
     </row>
     <row r="500" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="B500">
         <v>3011</v>
       </c>
       <c r="C500" t="s">
+        <v>2651</v>
+      </c>
+      <c r="J500" t="s">
         <v>2652</v>
-      </c>
-      <c r="J500" t="s">
-        <v>2653</v>
       </c>
       <c r="K500" t="s">
         <v>15</v>
@@ -23843,16 +23846,16 @@
     </row>
     <row r="632" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="B632">
         <v>3026</v>
       </c>
       <c r="C632" t="s">
+        <v>2654</v>
+      </c>
+      <c r="J632" t="s">
         <v>2655</v>
-      </c>
-      <c r="J632" t="s">
-        <v>2656</v>
       </c>
       <c r="K632" t="s">
         <v>15</v>
@@ -24472,16 +24475,16 @@
     </row>
     <row r="657" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
       <c r="B657">
         <v>3031</v>
       </c>
       <c r="C657" t="s">
+        <v>2657</v>
+      </c>
+      <c r="J657" t="s">
         <v>2658</v>
-      </c>
-      <c r="J657" t="s">
-        <v>2659</v>
       </c>
       <c r="K657" t="s">
         <v>15</v>
@@ -24492,16 +24495,16 @@
     </row>
     <row r="658" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="B658">
         <v>3032</v>
       </c>
       <c r="C658" t="s">
+        <v>2660</v>
+      </c>
+      <c r="J658" t="s">
         <v>2661</v>
-      </c>
-      <c r="J658" t="s">
-        <v>2662</v>
       </c>
       <c r="K658" t="s">
         <v>15</v>
@@ -24512,25 +24515,25 @@
     </row>
     <row r="659" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="B659">
         <v>118</v>
       </c>
       <c r="C659" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="D659" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="F659">
         <v>40</v>
       </c>
       <c r="G659" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="J659" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
       <c r="K659" t="s">
         <v>31</v>
@@ -24541,25 +24544,25 @@
     </row>
     <row r="660" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
       <c r="B660">
         <v>819</v>
       </c>
       <c r="C660" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
       <c r="D660" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
       <c r="F660">
         <v>40</v>
       </c>
       <c r="G660" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="J660" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
       <c r="K660" t="s">
         <v>31</v>
@@ -24570,22 +24573,22 @@
     </row>
     <row r="661" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
       <c r="B661">
         <v>312</v>
       </c>
       <c r="C661" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="D661" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
       <c r="F661">
         <v>40</v>
       </c>
       <c r="J661" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="K661" t="s">
         <v>31</v>
@@ -24596,16 +24599,16 @@
     </row>
     <row r="662" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="B662">
         <v>3033</v>
       </c>
       <c r="C662" t="s">
+        <v>2672</v>
+      </c>
+      <c r="J662" t="s">
         <v>2673</v>
-      </c>
-      <c r="J662" t="s">
-        <v>2674</v>
       </c>
       <c r="K662" t="s">
         <v>15</v>
@@ -24616,16 +24619,16 @@
     </row>
     <row r="663" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="B663">
         <v>3034</v>
       </c>
       <c r="C663" t="s">
+        <v>2675</v>
+      </c>
+      <c r="J663" t="s">
         <v>2676</v>
-      </c>
-      <c r="J663" t="s">
-        <v>2677</v>
       </c>
       <c r="K663" t="s">
         <v>15</v>
@@ -24636,16 +24639,16 @@
     </row>
     <row r="664" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
       <c r="B664">
         <v>3035</v>
       </c>
       <c r="C664" t="s">
+        <v>2678</v>
+      </c>
+      <c r="J664" t="s">
         <v>2679</v>
-      </c>
-      <c r="J664" t="s">
-        <v>2680</v>
       </c>
       <c r="K664" t="s">
         <v>15</v>
@@ -24656,22 +24659,22 @@
     </row>
     <row r="665" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="B665">
         <v>1268</v>
       </c>
       <c r="C665" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="D665" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="F665">
         <v>40</v>
       </c>
       <c r="J665" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="K665" t="s">
         <v>31</v>
@@ -24751,16 +24754,16 @@
     </row>
     <row r="669" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="B669">
         <v>3039</v>
       </c>
       <c r="C669" t="s">
+        <v>2684</v>
+      </c>
+      <c r="J669" t="s">
         <v>2685</v>
-      </c>
-      <c r="J669" t="s">
-        <v>2686</v>
       </c>
       <c r="K669" t="s">
         <v>15</v>
@@ -24835,16 +24838,16 @@
     </row>
     <row r="672" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="B672">
         <v>1180</v>
       </c>
       <c r="C672" t="s">
-        <v>2688</v>
+        <v>2687</v>
       </c>
       <c r="D672" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="F672">
         <v>39</v>
@@ -24933,16 +24936,16 @@
     </row>
     <row r="676" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="B676">
         <v>3040</v>
       </c>
       <c r="C676" t="s">
+        <v>2689</v>
+      </c>
+      <c r="J676" t="s">
         <v>2690</v>
-      </c>
-      <c r="J676" t="s">
-        <v>2691</v>
       </c>
       <c r="K676" t="s">
         <v>15</v>
@@ -24999,16 +25002,16 @@
     </row>
     <row r="679" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="B679">
         <v>3041</v>
       </c>
       <c r="C679" t="s">
+        <v>2692</v>
+      </c>
+      <c r="J679" t="s">
         <v>2693</v>
-      </c>
-      <c r="J679" t="s">
-        <v>2694</v>
       </c>
       <c r="K679" t="s">
         <v>15</v>
@@ -25019,16 +25022,16 @@
     </row>
     <row r="680" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="B680">
         <v>3042</v>
       </c>
       <c r="C680" t="s">
+        <v>2695</v>
+      </c>
+      <c r="J680" t="s">
         <v>2696</v>
-      </c>
-      <c r="J680" t="s">
-        <v>2697</v>
       </c>
       <c r="K680" t="s">
         <v>15</v>
@@ -25062,16 +25065,16 @@
     </row>
     <row r="682" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="B682">
         <v>3043</v>
       </c>
       <c r="C682" t="s">
+        <v>2698</v>
+      </c>
+      <c r="J682" t="s">
         <v>2699</v>
-      </c>
-      <c r="J682" t="s">
-        <v>2700</v>
       </c>
       <c r="K682" t="s">
         <v>15</v>
@@ -25105,16 +25108,16 @@
     </row>
     <row r="684" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="B684">
         <v>3044</v>
       </c>
       <c r="C684" t="s">
+        <v>2701</v>
+      </c>
+      <c r="J684" t="s">
         <v>2702</v>
-      </c>
-      <c r="J684" t="s">
-        <v>2703</v>
       </c>
       <c r="K684" t="s">
         <v>15</v>
@@ -25125,16 +25128,16 @@
     </row>
     <row r="685" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="B685">
         <v>3047</v>
       </c>
       <c r="C685" t="s">
+        <v>2704</v>
+      </c>
+      <c r="J685" t="s">
         <v>2705</v>
-      </c>
-      <c r="J685" t="s">
-        <v>2706</v>
       </c>
       <c r="K685" t="s">
         <v>15</v>
@@ -25145,16 +25148,16 @@
     </row>
     <row r="686" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="B686">
         <v>321</v>
       </c>
       <c r="C686" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="D686" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="F686">
         <v>40</v>
@@ -25171,22 +25174,22 @@
     </row>
     <row r="687" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="B687">
         <v>1334</v>
       </c>
       <c r="C687" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="D687" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="F687">
         <v>40</v>
       </c>
       <c r="J687" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="K687" t="s">
         <v>31</v>
@@ -25358,16 +25361,16 @@
     </row>
     <row r="695" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="B695">
         <v>3048</v>
       </c>
       <c r="C695" t="s">
+        <v>2712</v>
+      </c>
+      <c r="J695" t="s">
         <v>2713</v>
-      </c>
-      <c r="J695" t="s">
-        <v>2714</v>
       </c>
       <c r="K695" t="s">
         <v>15</v>
@@ -25401,16 +25404,16 @@
     </row>
     <row r="697" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="B697">
         <v>3049</v>
       </c>
       <c r="C697" t="s">
+        <v>2715</v>
+      </c>
+      <c r="J697" t="s">
         <v>2716</v>
-      </c>
-      <c r="J697" t="s">
-        <v>2717</v>
       </c>
       <c r="K697" t="s">
         <v>15</v>
@@ -25421,16 +25424,16 @@
     </row>
     <row r="698" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="B698">
         <v>3050</v>
       </c>
       <c r="C698" t="s">
+        <v>2718</v>
+      </c>
+      <c r="J698" t="s">
         <v>2719</v>
-      </c>
-      <c r="J698" t="s">
-        <v>2720</v>
       </c>
       <c r="K698" t="s">
         <v>15</v>
@@ -25441,16 +25444,16 @@
     </row>
     <row r="699" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="B699">
         <v>3051</v>
       </c>
       <c r="C699" t="s">
+        <v>2721</v>
+      </c>
+      <c r="J699" t="s">
         <v>2722</v>
-      </c>
-      <c r="J699" t="s">
-        <v>2723</v>
       </c>
       <c r="K699" t="s">
         <v>15</v>
@@ -25507,16 +25510,16 @@
     </row>
     <row r="702" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="B702">
         <v>3052</v>
       </c>
       <c r="C702" t="s">
+        <v>2724</v>
+      </c>
+      <c r="J702" t="s">
         <v>2725</v>
-      </c>
-      <c r="J702" t="s">
-        <v>2726</v>
       </c>
       <c r="K702" t="s">
         <v>15</v>
@@ -25556,10 +25559,10 @@
         <v>3053</v>
       </c>
       <c r="C704" t="s">
+        <v>2726</v>
+      </c>
+      <c r="J704" t="s">
         <v>2727</v>
-      </c>
-      <c r="J704" t="s">
-        <v>2728</v>
       </c>
       <c r="K704" t="s">
         <v>15</v>
@@ -26714,16 +26717,16 @@
     </row>
     <row r="755" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="B755">
         <v>3058</v>
       </c>
       <c r="C755" t="s">
+        <v>2729</v>
+      </c>
+      <c r="J755" t="s">
         <v>2730</v>
-      </c>
-      <c r="J755" t="s">
-        <v>2731</v>
       </c>
       <c r="K755" t="s">
         <v>15</v>
@@ -26734,22 +26737,22 @@
     </row>
     <row r="756" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="B756">
         <v>141</v>
       </c>
       <c r="C756" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="D756" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="F756">
         <v>38</v>
       </c>
       <c r="J756" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="K756" t="s">
         <v>31</v>
@@ -26760,16 +26763,16 @@
     </row>
     <row r="757" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="B757">
         <v>3059</v>
       </c>
       <c r="C757" t="s">
+        <v>2735</v>
+      </c>
+      <c r="J757" t="s">
         <v>2736</v>
-      </c>
-      <c r="J757" t="s">
-        <v>2737</v>
       </c>
       <c r="K757" t="s">
         <v>15</v>
@@ -26780,22 +26783,22 @@
     </row>
     <row r="758" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="B758">
         <v>191</v>
       </c>
       <c r="C758" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="D758" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="F758">
         <v>38</v>
       </c>
       <c r="J758" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="K758" t="s">
         <v>31</v>
@@ -26806,16 +26809,16 @@
     </row>
     <row r="759" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="B759">
         <v>3060</v>
       </c>
       <c r="C759" t="s">
+        <v>2741</v>
+      </c>
+      <c r="J759" t="s">
         <v>2742</v>
-      </c>
-      <c r="J759" t="s">
-        <v>2743</v>
       </c>
       <c r="K759" t="s">
         <v>15</v>
@@ -26826,19 +26829,19 @@
     </row>
     <row r="760" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
       <c r="B760">
         <v>2290</v>
       </c>
       <c r="C760" t="s">
+        <v>2744</v>
+      </c>
+      <c r="I760" t="s">
+        <v>2743</v>
+      </c>
+      <c r="J760" t="s">
         <v>2745</v>
-      </c>
-      <c r="I760" t="s">
-        <v>2744</v>
-      </c>
-      <c r="J760" t="s">
-        <v>2746</v>
       </c>
       <c r="K760" t="s">
         <v>31</v>
@@ -26855,7 +26858,7 @@
         <v>3061</v>
       </c>
       <c r="C761" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="J761" t="s">
         <v>1350</v>
@@ -27273,16 +27276,16 @@
     </row>
     <row r="781" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="B781">
         <v>3068</v>
       </c>
       <c r="C781" t="s">
+        <v>2748</v>
+      </c>
+      <c r="J781" t="s">
         <v>2749</v>
-      </c>
-      <c r="J781" t="s">
-        <v>2750</v>
       </c>
       <c r="K781" t="s">
         <v>15</v>
@@ -27293,16 +27296,16 @@
     </row>
     <row r="782" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="B782">
         <v>1330</v>
       </c>
       <c r="C782" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="D782" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="F782">
         <v>40</v>
@@ -27486,16 +27489,16 @@
     </row>
     <row r="790" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="B790">
         <v>3071</v>
       </c>
       <c r="C790" t="s">
+        <v>2753</v>
+      </c>
+      <c r="J790" t="s">
         <v>2754</v>
-      </c>
-      <c r="J790" t="s">
-        <v>2755</v>
       </c>
       <c r="K790" t="s">
         <v>15</v>
@@ -27506,22 +27509,22 @@
     </row>
     <row r="791" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="B791">
         <v>1195</v>
       </c>
       <c r="C791" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="D791" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="F791">
         <v>40</v>
       </c>
       <c r="J791" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="K791" t="s">
         <v>31</v>
@@ -27538,7 +27541,7 @@
         <v>83</v>
       </c>
       <c r="C792" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="D792" t="s">
         <v>992</v>
@@ -27550,7 +27553,7 @@
         <v>992</v>
       </c>
       <c r="J792" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="K792" t="s">
         <v>31</v>
@@ -27561,22 +27564,22 @@
     </row>
     <row r="793" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="B793">
         <v>972</v>
       </c>
       <c r="C793" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="D793" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="F793">
         <v>40</v>
       </c>
       <c r="J793" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="K793" t="s">
         <v>31</v>
@@ -27587,16 +27590,16 @@
     </row>
     <row r="794" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="B794">
         <v>3072</v>
       </c>
       <c r="C794" t="s">
+        <v>2763</v>
+      </c>
+      <c r="J794" t="s">
         <v>2764</v>
-      </c>
-      <c r="J794" t="s">
-        <v>2765</v>
       </c>
       <c r="K794" t="s">
         <v>15</v>
@@ -27607,22 +27610,22 @@
     </row>
     <row r="795" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="B795">
         <v>939</v>
       </c>
       <c r="C795" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="D795" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="F795">
         <v>40</v>
       </c>
       <c r="J795" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="K795" t="s">
         <v>31</v>
@@ -28957,16 +28960,16 @@
     </row>
     <row r="855" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="B855">
         <v>3102</v>
       </c>
       <c r="C855" t="s">
+        <v>2769</v>
+      </c>
+      <c r="J855" t="s">
         <v>2770</v>
-      </c>
-      <c r="J855" t="s">
-        <v>2771</v>
       </c>
       <c r="K855" t="s">
         <v>15</v>
@@ -28977,16 +28980,16 @@
     </row>
     <row r="856" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="B856">
         <v>3103</v>
       </c>
       <c r="C856" t="s">
+        <v>2772</v>
+      </c>
+      <c r="J856" t="s">
         <v>2773</v>
-      </c>
-      <c r="J856" t="s">
-        <v>2774</v>
       </c>
       <c r="K856" t="s">
         <v>15</v>
@@ -29245,16 +29248,16 @@
     </row>
     <row r="867" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="B867">
         <v>3106</v>
       </c>
       <c r="C867" t="s">
+        <v>2775</v>
+      </c>
+      <c r="J867" t="s">
         <v>2776</v>
-      </c>
-      <c r="J867" t="s">
-        <v>2777</v>
       </c>
       <c r="K867" t="s">
         <v>15</v>
@@ -29265,22 +29268,22 @@
     </row>
     <row r="868" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="B868">
         <v>1214</v>
       </c>
       <c r="C868" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="D868" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="F868">
         <v>40</v>
       </c>
       <c r="J868" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="K868" t="s">
         <v>31</v>
@@ -29291,22 +29294,22 @@
     </row>
     <row r="869" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="B869">
         <v>1296</v>
       </c>
       <c r="C869" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="D869" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="F869">
         <v>40</v>
       </c>
       <c r="J869" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="K869" t="s">
         <v>31</v>
@@ -30218,16 +30221,16 @@
     </row>
     <row r="911" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A911" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="B911">
         <v>3136</v>
       </c>
       <c r="C911" t="s">
+        <v>2784</v>
+      </c>
+      <c r="J911" t="s">
         <v>2785</v>
-      </c>
-      <c r="J911" t="s">
-        <v>2786</v>
       </c>
       <c r="K911" t="s">
         <v>31</v>
@@ -30330,13 +30333,13 @@
     </row>
     <row r="916" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="B916">
         <v>3139</v>
       </c>
       <c r="C916" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="K916" t="s">
         <v>31</v>
@@ -30373,13 +30376,13 @@
     </row>
     <row r="918" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A918" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="B918">
         <v>3140</v>
       </c>
       <c r="C918" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="K918" t="s">
         <v>31</v>
@@ -30784,16 +30787,16 @@
     </row>
     <row r="936" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A936" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="B936">
         <v>3151</v>
       </c>
       <c r="C936" t="s">
+        <v>2791</v>
+      </c>
+      <c r="J936" t="s">
         <v>2792</v>
-      </c>
-      <c r="J936" t="s">
-        <v>2793</v>
       </c>
       <c r="K936" t="s">
         <v>31</v>
@@ -33031,16 +33034,16 @@
     </row>
     <row r="1032" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1032" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="B1032">
         <v>3206</v>
       </c>
       <c r="C1032" t="s">
+        <v>2794</v>
+      </c>
+      <c r="J1032" t="s">
         <v>2795</v>
-      </c>
-      <c r="J1032" t="s">
-        <v>2796</v>
       </c>
       <c r="K1032" t="s">
         <v>31</v>
@@ -33051,16 +33054,16 @@
     </row>
     <row r="1033" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1033" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="B1033">
         <v>3207</v>
       </c>
       <c r="C1033" t="s">
+        <v>2797</v>
+      </c>
+      <c r="J1033" t="s">
         <v>2798</v>
-      </c>
-      <c r="J1033" t="s">
-        <v>2799</v>
       </c>
       <c r="K1033" t="s">
         <v>31</v>
@@ -33071,13 +33074,13 @@
     </row>
     <row r="1034" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1034" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="B1034">
         <v>3208</v>
       </c>
       <c r="C1034" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="K1034" t="s">
         <v>31</v>
@@ -33088,16 +33091,16 @@
     </row>
     <row r="1035" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1035" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="B1035">
         <v>3209</v>
       </c>
       <c r="C1035" t="s">
+        <v>2802</v>
+      </c>
+      <c r="J1035" t="s">
         <v>2803</v>
-      </c>
-      <c r="J1035" t="s">
-        <v>2804</v>
       </c>
       <c r="K1035" t="s">
         <v>31</v>
@@ -33108,16 +33111,16 @@
     </row>
     <row r="1036" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1036" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="B1036">
         <v>3210</v>
       </c>
       <c r="C1036" t="s">
+        <v>2805</v>
+      </c>
+      <c r="J1036" t="s">
         <v>2806</v>
-      </c>
-      <c r="J1036" t="s">
-        <v>2807</v>
       </c>
       <c r="K1036" t="s">
         <v>31</v>
@@ -33128,13 +33131,13 @@
     </row>
     <row r="1037" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1037" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="B1037">
         <v>3211</v>
       </c>
       <c r="C1037" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="J1037" t="s">
         <v>2323</v>
@@ -33573,16 +33576,16 @@
     </row>
     <row r="1057" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1057" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="B1057">
         <v>3223</v>
       </c>
       <c r="C1057" t="s">
+        <v>2810</v>
+      </c>
+      <c r="J1057" t="s">
         <v>2811</v>
-      </c>
-      <c r="J1057" t="s">
-        <v>2812</v>
       </c>
       <c r="K1057" t="s">
         <v>15</v>
@@ -33593,16 +33596,16 @@
     </row>
     <row r="1058" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1058" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="B1058">
         <v>3224</v>
       </c>
       <c r="C1058" t="s">
+        <v>2813</v>
+      </c>
+      <c r="J1058" t="s">
         <v>2814</v>
-      </c>
-      <c r="J1058" t="s">
-        <v>2815</v>
       </c>
       <c r="K1058" t="s">
         <v>15</v>
@@ -33613,16 +33616,16 @@
     </row>
     <row r="1059" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1059" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="B1059">
         <v>3225</v>
       </c>
       <c r="C1059" t="s">
+        <v>2816</v>
+      </c>
+      <c r="J1059" t="s">
         <v>2817</v>
-      </c>
-      <c r="J1059" t="s">
-        <v>2818</v>
       </c>
       <c r="K1059" t="s">
         <v>15</v>
@@ -33633,22 +33636,22 @@
     </row>
     <row r="1060" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1060" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="B1060">
         <v>434</v>
       </c>
       <c r="C1060" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="D1060" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="F1060">
         <v>40</v>
       </c>
       <c r="J1060" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="K1060" t="s">
         <v>31</v>

</xml_diff>